<commit_message>
Update Every Snes Game (US_EU) - GMDQ.xlsx
Adds publisher
</commit_message>
<xml_diff>
--- a/snes/Every Snes Game (US_EU) - GMDQ.xlsx
+++ b/snes/Every Snes Game (US_EU) - GMDQ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\2kgames.t2.corp\Network\2KGCZE\ToolTeam\Tableau\GitHub\103percent\GamesOnSpreadsheets\GamesOnSpreadsheets\snes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8ADA2A-D16C-4783-ACC2-B2F515BB4FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF80F20E-F15D-4A78-9ECE-C72DC731D6E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1365" yWindow="1650" windowWidth="35235" windowHeight="18300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2321" uniqueCount="1109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2323" uniqueCount="1111">
   <si>
     <t>Title</t>
   </si>
@@ -3348,6 +3348,12 @@
   </si>
   <si>
     <t>Chris Scullion</t>
+  </si>
+  <si>
+    <t>Publisher</t>
+  </si>
+  <si>
+    <t>White Owl</t>
   </si>
 </sst>
 </file>
@@ -14453,10 +14459,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B2C521-58EE-4225-A514-0523230A0C72}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14465,10 +14471,11 @@
     <col min="2" max="2" width="24.7109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="43.5703125" style="3" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="3"/>
+    <col min="5" max="5" width="17.5703125" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>1103</v>
       </c>
@@ -14481,8 +14488,11 @@
       <c r="D1" s="5" t="s">
         <v>1105</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E1" s="5" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -14494,6 +14504,9 @@
       </c>
       <c r="D2" s="4" t="s">
         <v>1108</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>1110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>